<commit_message>
Se creó la función optimización para poder reutilizarla en diferentes puntos de código y se creó la funcionalidad de encontrar las franjas iniciales del almuerzo
</commit_message>
<xml_diff>
--- a/src/PuLP/solucionOptima.xlsx
+++ b/src/PuLP/solucionOptima.xlsx
@@ -510,7 +510,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F3" t="n">
@@ -536,7 +536,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F4" t="n">
@@ -562,7 +562,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F5" t="n">
@@ -978,7 +978,7 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F21" t="n">
@@ -1004,7 +1004,7 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F22" t="n">
@@ -1030,7 +1030,7 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F23" t="n">
@@ -1108,7 +1108,7 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F26" t="n">
@@ -1160,7 +1160,7 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F28" t="n">
@@ -1238,7 +1238,7 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F31" t="n">
@@ -1446,7 +1446,7 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F39" t="n">
@@ -1550,7 +1550,7 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F43" t="n">
@@ -1602,7 +1602,7 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F45" t="n">
@@ -1628,7 +1628,7 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F46" t="n">
@@ -1654,7 +1654,7 @@
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F47" t="n">
@@ -1732,7 +1732,7 @@
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F50" t="n">
@@ -2096,7 +2096,7 @@
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F64" t="n">
@@ -2122,7 +2122,7 @@
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F65" t="n">
@@ -2148,7 +2148,7 @@
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F66" t="n">
@@ -2174,7 +2174,7 @@
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F67" t="n">
@@ -2252,7 +2252,7 @@
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F70" t="n">
@@ -2330,7 +2330,7 @@
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F73" t="n">
@@ -2408,7 +2408,7 @@
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F76" t="n">
@@ -2434,7 +2434,7 @@
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F77" t="n">
@@ -2512,7 +2512,7 @@
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F80" t="n">
@@ -2538,7 +2538,7 @@
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F81" t="n">
@@ -2642,7 +2642,7 @@
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F85" t="n">
@@ -2668,7 +2668,7 @@
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F86" t="n">
@@ -2772,7 +2772,7 @@
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F90" t="n">
@@ -2798,7 +2798,7 @@
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F91" t="n">
@@ -2850,7 +2850,7 @@
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F93" t="n">
@@ -2928,7 +2928,7 @@
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F96" t="n">
@@ -3084,7 +3084,7 @@
       </c>
       <c r="E102" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F102" t="n">
@@ -3292,7 +3292,7 @@
       </c>
       <c r="E110" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F110" t="n">
@@ -3370,7 +3370,7 @@
       </c>
       <c r="E113" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F113" t="n">
@@ -3396,7 +3396,7 @@
       </c>
       <c r="E114" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F114" t="n">
@@ -3578,7 +3578,7 @@
       </c>
       <c r="E121" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F121" t="n">
@@ -3604,7 +3604,7 @@
       </c>
       <c r="E122" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F122" t="n">
@@ -3630,7 +3630,7 @@
       </c>
       <c r="E123" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F123" t="n">
@@ -3708,7 +3708,7 @@
       </c>
       <c r="E126" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F126" t="n">
@@ -3838,7 +3838,7 @@
       </c>
       <c r="E131" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F131" t="n">
@@ -3864,7 +3864,7 @@
       </c>
       <c r="E132" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F132" t="n">
@@ -3890,7 +3890,7 @@
       </c>
       <c r="E133" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F133" t="n">
@@ -3916,7 +3916,7 @@
       </c>
       <c r="E134" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F134" t="n">
@@ -3942,7 +3942,7 @@
       </c>
       <c r="E135" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F135" t="n">
@@ -3968,7 +3968,7 @@
       </c>
       <c r="E136" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F136" t="n">
@@ -4020,7 +4020,7 @@
       </c>
       <c r="E138" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F138" t="n">
@@ -4072,7 +4072,7 @@
       </c>
       <c r="E140" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F140" t="n">
@@ -4098,7 +4098,7 @@
       </c>
       <c r="E141" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F141" t="n">
@@ -4488,7 +4488,7 @@
       </c>
       <c r="E156" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F156" t="n">
@@ -4540,7 +4540,7 @@
       </c>
       <c r="E158" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F158" t="n">
@@ -4618,7 +4618,7 @@
       </c>
       <c r="E161" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F161" t="n">
@@ -4774,7 +4774,7 @@
       </c>
       <c r="E167" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F167" t="n">
@@ -4800,7 +4800,7 @@
       </c>
       <c r="E168" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F168" t="n">
@@ -4826,7 +4826,7 @@
       </c>
       <c r="E169" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F169" t="n">
@@ -4904,7 +4904,7 @@
       </c>
       <c r="E172" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F172" t="n">
@@ -4930,7 +4930,7 @@
       </c>
       <c r="E173" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F173" t="n">
@@ -4956,7 +4956,7 @@
       </c>
       <c r="E174" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F174" t="n">
@@ -5190,7 +5190,7 @@
       </c>
       <c r="E183" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F183" t="n">
@@ -5216,7 +5216,7 @@
       </c>
       <c r="E184" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F184" t="n">
@@ -5242,7 +5242,7 @@
       </c>
       <c r="E185" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F185" t="n">
@@ -5294,7 +5294,7 @@
       </c>
       <c r="E187" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F187" t="n">
@@ -5320,7 +5320,7 @@
       </c>
       <c r="E188" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F188" t="n">
@@ -5710,7 +5710,7 @@
       </c>
       <c r="E203" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F203" t="n">
@@ -5736,7 +5736,7 @@
       </c>
       <c r="E204" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F204" t="n">
@@ -5814,7 +5814,7 @@
       </c>
       <c r="E207" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F207" t="n">
@@ -5866,7 +5866,7 @@
       </c>
       <c r="E209" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F209" t="n">
@@ -5892,7 +5892,7 @@
       </c>
       <c r="E210" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F210" t="n">
@@ -5970,7 +5970,7 @@
       </c>
       <c r="E213" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F213" t="n">
@@ -6100,7 +6100,7 @@
       </c>
       <c r="E218" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F218" t="n">
@@ -6126,7 +6126,7 @@
       </c>
       <c r="E219" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F219" t="n">
@@ -6152,7 +6152,7 @@
       </c>
       <c r="E220" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F220" t="n">
@@ -6256,7 +6256,7 @@
       </c>
       <c r="E224" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F224" t="n">
@@ -6334,7 +6334,7 @@
       </c>
       <c r="E227" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F227" t="n">
@@ -6438,7 +6438,7 @@
       </c>
       <c r="E231" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F231" t="n">
@@ -6516,7 +6516,7 @@
       </c>
       <c r="E234" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F234" t="n">
@@ -6542,7 +6542,7 @@
       </c>
       <c r="E235" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F235" t="n">
@@ -6932,7 +6932,7 @@
       </c>
       <c r="E250" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F250" t="n">
@@ -6984,7 +6984,7 @@
       </c>
       <c r="E252" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F252" t="n">
@@ -7010,7 +7010,7 @@
       </c>
       <c r="E253" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F253" t="n">
@@ -7062,7 +7062,7 @@
       </c>
       <c r="E255" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F255" t="n">
@@ -7140,7 +7140,7 @@
       </c>
       <c r="E258" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F258" t="n">
@@ -7218,7 +7218,7 @@
       </c>
       <c r="E261" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F261" t="n">
@@ -7348,7 +7348,7 @@
       </c>
       <c r="E266" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F266" t="n">
@@ -7374,7 +7374,7 @@
       </c>
       <c r="E267" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F267" t="n">
@@ -7426,7 +7426,7 @@
       </c>
       <c r="E269" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F269" t="n">
@@ -7478,7 +7478,7 @@
       </c>
       <c r="E271" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F271" t="n">
@@ -7530,7 +7530,7 @@
       </c>
       <c r="E273" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F273" t="n">
@@ -7582,7 +7582,7 @@
       </c>
       <c r="E275" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F275" t="n">
@@ -7712,7 +7712,7 @@
       </c>
       <c r="E280" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F280" t="n">
@@ -8076,7 +8076,7 @@
       </c>
       <c r="E294" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F294" t="n">
@@ -8128,7 +8128,7 @@
       </c>
       <c r="E296" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F296" t="n">
@@ -8154,7 +8154,7 @@
       </c>
       <c r="E297" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F297" t="n">
@@ -8206,7 +8206,7 @@
       </c>
       <c r="E299" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F299" t="n">
@@ -8258,7 +8258,7 @@
       </c>
       <c r="E301" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F301" t="n">
@@ -8284,7 +8284,7 @@
       </c>
       <c r="E302" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F302" t="n">
@@ -8310,7 +8310,7 @@
       </c>
       <c r="E303" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F303" t="n">
@@ -8388,7 +8388,7 @@
       </c>
       <c r="E306" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F306" t="n">
@@ -8492,7 +8492,7 @@
       </c>
       <c r="E310" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F310" t="n">
@@ -8518,7 +8518,7 @@
       </c>
       <c r="E311" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F311" t="n">
@@ -8570,7 +8570,7 @@
       </c>
       <c r="E313" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F313" t="n">
@@ -8622,7 +8622,7 @@
       </c>
       <c r="E315" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F315" t="n">
@@ -8752,7 +8752,7 @@
       </c>
       <c r="E320" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F320" t="n">
@@ -8856,7 +8856,7 @@
       </c>
       <c r="E324" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F324" t="n">
@@ -8882,7 +8882,7 @@
       </c>
       <c r="E325" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F325" t="n">
@@ -9064,7 +9064,7 @@
       </c>
       <c r="E332" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F332" t="n">
@@ -9272,7 +9272,7 @@
       </c>
       <c r="E340" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F340" t="n">
@@ -9324,7 +9324,7 @@
       </c>
       <c r="E342" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F342" t="n">
@@ -9350,7 +9350,7 @@
       </c>
       <c r="E343" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F343" t="n">
@@ -9376,7 +9376,7 @@
       </c>
       <c r="E344" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F344" t="n">
@@ -9428,7 +9428,7 @@
       </c>
       <c r="E346" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F346" t="n">
@@ -9454,7 +9454,7 @@
       </c>
       <c r="E347" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F347" t="n">
@@ -9480,7 +9480,7 @@
       </c>
       <c r="E348" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F348" t="n">
@@ -9506,7 +9506,7 @@
       </c>
       <c r="E349" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F349" t="n">
@@ -9532,7 +9532,7 @@
       </c>
       <c r="E350" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F350" t="n">
@@ -9584,7 +9584,7 @@
       </c>
       <c r="E352" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F352" t="n">
@@ -9688,7 +9688,7 @@
       </c>
       <c r="E356" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F356" t="n">
@@ -9740,7 +9740,7 @@
       </c>
       <c r="E358" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F358" t="n">
@@ -9818,7 +9818,7 @@
       </c>
       <c r="E361" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F361" t="n">
@@ -9844,7 +9844,7 @@
       </c>
       <c r="E362" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F362" t="n">
@@ -9896,7 +9896,7 @@
       </c>
       <c r="E364" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F364" t="n">
@@ -9948,7 +9948,7 @@
       </c>
       <c r="E366" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F366" t="n">
@@ -10000,7 +10000,7 @@
       </c>
       <c r="E368" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F368" t="n">

</xml_diff>

<commit_message>
Se agregaron mas restricciones al modelo
</commit_message>
<xml_diff>
--- a/src/PuLP/solucionOptima.xlsx
+++ b/src/PuLP/solucionOptima.xlsx
@@ -510,7 +510,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F3" t="n">
@@ -562,7 +562,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F5" t="n">
@@ -588,7 +588,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F6" t="n">
@@ -614,7 +614,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F7" t="n">
@@ -640,7 +640,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F8" t="n">
@@ -666,7 +666,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F9" t="n">
@@ -1342,7 +1342,7 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F35" t="n">
@@ -1368,7 +1368,7 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F36" t="n">
@@ -1446,7 +1446,7 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F39" t="n">
@@ -1472,7 +1472,7 @@
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F40" t="n">
@@ -1524,7 +1524,7 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F42" t="n">
@@ -1576,7 +1576,7 @@
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F44" t="n">
@@ -1602,7 +1602,7 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F45" t="n">
@@ -1628,7 +1628,7 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F46" t="n">
@@ -1732,7 +1732,7 @@
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F50" t="n">
@@ -1758,7 +1758,7 @@
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F51" t="n">
@@ -1784,7 +1784,7 @@
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F52" t="n">
@@ -1810,7 +1810,7 @@
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F53" t="n">
@@ -1836,7 +1836,7 @@
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F54" t="n">
@@ -1862,7 +1862,7 @@
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F55" t="n">
@@ -2538,7 +2538,7 @@
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F81" t="n">
@@ -2564,7 +2564,7 @@
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F82" t="n">
@@ -2642,7 +2642,7 @@
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F85" t="n">
@@ -2720,7 +2720,7 @@
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F88" t="n">
@@ -2798,7 +2798,7 @@
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F91" t="n">
@@ -2824,7 +2824,7 @@
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F92" t="n">
@@ -2850,7 +2850,7 @@
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F93" t="n">
@@ -2876,7 +2876,7 @@
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F94" t="n">
@@ -2928,7 +2928,7 @@
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F96" t="n">
@@ -2954,7 +2954,7 @@
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F97" t="n">
@@ -2980,7 +2980,7 @@
       </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F98" t="n">
@@ -3006,7 +3006,7 @@
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F99" t="n">
@@ -3032,7 +3032,7 @@
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F100" t="n">
@@ -3058,7 +3058,7 @@
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F101" t="n">
@@ -3734,7 +3734,7 @@
       </c>
       <c r="E127" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F127" t="n">
@@ -3838,7 +3838,7 @@
       </c>
       <c r="E131" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F131" t="n">
@@ -3890,7 +3890,7 @@
       </c>
       <c r="E133" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F133" t="n">
@@ -3916,7 +3916,7 @@
       </c>
       <c r="E134" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F134" t="n">
@@ -3968,7 +3968,7 @@
       </c>
       <c r="E136" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F136" t="n">
@@ -3994,7 +3994,7 @@
       </c>
       <c r="E137" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F137" t="n">
@@ -4020,7 +4020,7 @@
       </c>
       <c r="E138" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F138" t="n">
@@ -4046,7 +4046,7 @@
       </c>
       <c r="E139" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F139" t="n">
@@ -4124,7 +4124,7 @@
       </c>
       <c r="E142" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F142" t="n">
@@ -4150,7 +4150,7 @@
       </c>
       <c r="E143" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F143" t="n">
@@ -4176,7 +4176,7 @@
       </c>
       <c r="E144" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F144" t="n">
@@ -4202,7 +4202,7 @@
       </c>
       <c r="E145" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F145" t="n">
@@ -4228,7 +4228,7 @@
       </c>
       <c r="E146" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F146" t="n">
@@ -4254,7 +4254,7 @@
       </c>
       <c r="E147" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F147" t="n">
@@ -4280,7 +4280,7 @@
       </c>
       <c r="E148" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F148" t="n">
@@ -4904,7 +4904,7 @@
       </c>
       <c r="E172" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F172" t="n">
@@ -5060,7 +5060,7 @@
       </c>
       <c r="E178" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F178" t="n">
@@ -5086,7 +5086,7 @@
       </c>
       <c r="E179" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F179" t="n">
@@ -5138,7 +5138,7 @@
       </c>
       <c r="E181" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F181" t="n">
@@ -5164,7 +5164,7 @@
       </c>
       <c r="E182" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F182" t="n">
@@ -5294,7 +5294,7 @@
       </c>
       <c r="E187" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F187" t="n">
@@ -5346,7 +5346,7 @@
       </c>
       <c r="E189" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F189" t="n">
@@ -5372,7 +5372,7 @@
       </c>
       <c r="E190" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F190" t="n">
@@ -5398,7 +5398,7 @@
       </c>
       <c r="E191" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F191" t="n">
@@ -5424,7 +5424,7 @@
       </c>
       <c r="E192" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F192" t="n">
@@ -5450,7 +5450,7 @@
       </c>
       <c r="E193" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F193" t="n">
@@ -6100,7 +6100,7 @@
       </c>
       <c r="E218" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F218" t="n">
@@ -6230,7 +6230,7 @@
       </c>
       <c r="E223" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F223" t="n">
@@ -6256,7 +6256,7 @@
       </c>
       <c r="E224" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F224" t="n">
@@ -6334,7 +6334,7 @@
       </c>
       <c r="E227" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F227" t="n">
@@ -6360,7 +6360,7 @@
       </c>
       <c r="E228" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F228" t="n">
@@ -6386,7 +6386,7 @@
       </c>
       <c r="E229" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F229" t="n">
@@ -6412,7 +6412,7 @@
       </c>
       <c r="E230" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F230" t="n">
@@ -6438,7 +6438,7 @@
       </c>
       <c r="E231" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F231" t="n">
@@ -6568,7 +6568,7 @@
       </c>
       <c r="E236" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F236" t="n">
@@ -6594,7 +6594,7 @@
       </c>
       <c r="E237" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F237" t="n">
@@ -6620,7 +6620,7 @@
       </c>
       <c r="E238" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F238" t="n">
@@ -6646,7 +6646,7 @@
       </c>
       <c r="E239" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F239" t="n">
@@ -7296,7 +7296,7 @@
       </c>
       <c r="E264" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F264" t="n">
@@ -7374,7 +7374,7 @@
       </c>
       <c r="E267" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F267" t="n">
@@ -7478,7 +7478,7 @@
       </c>
       <c r="E271" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F271" t="n">
@@ -7504,7 +7504,7 @@
       </c>
       <c r="E272" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F272" t="n">
@@ -7556,7 +7556,7 @@
       </c>
       <c r="E274" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F274" t="n">
@@ -7608,7 +7608,7 @@
       </c>
       <c r="E276" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F276" t="n">
@@ -7634,7 +7634,7 @@
       </c>
       <c r="E277" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F277" t="n">
@@ -7712,7 +7712,7 @@
       </c>
       <c r="E280" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F280" t="n">
@@ -7738,7 +7738,7 @@
       </c>
       <c r="E281" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F281" t="n">
@@ -7764,7 +7764,7 @@
       </c>
       <c r="E282" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F282" t="n">
@@ -7790,7 +7790,7 @@
       </c>
       <c r="E283" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F283" t="n">
@@ -7816,7 +7816,7 @@
       </c>
       <c r="E284" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F284" t="n">
@@ -7842,7 +7842,7 @@
       </c>
       <c r="E285" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F285" t="n">
@@ -8544,7 +8544,7 @@
       </c>
       <c r="E312" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F312" t="n">
@@ -8570,7 +8570,7 @@
       </c>
       <c r="E313" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F313" t="n">
@@ -8752,7 +8752,7 @@
       </c>
       <c r="E320" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F320" t="n">
@@ -8778,7 +8778,7 @@
       </c>
       <c r="E321" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F321" t="n">
@@ -8804,7 +8804,7 @@
       </c>
       <c r="E322" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F322" t="n">
@@ -8830,7 +8830,7 @@
       </c>
       <c r="E323" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F323" t="n">
@@ -8882,7 +8882,7 @@
       </c>
       <c r="E325" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F325" t="n">
@@ -8908,7 +8908,7 @@
       </c>
       <c r="E326" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F326" t="n">
@@ -9688,7 +9688,7 @@
       </c>
       <c r="E356" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F356" t="n">
@@ -9714,7 +9714,7 @@
       </c>
       <c r="E357" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F357" t="n">
@@ -9740,7 +9740,7 @@
       </c>
       <c r="E358" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F358" t="n">
@@ -9844,7 +9844,7 @@
       </c>
       <c r="E362" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F362" t="n">
@@ -9948,7 +9948,7 @@
       </c>
       <c r="E366" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F366" t="n">
@@ -10000,7 +10000,7 @@
       </c>
       <c r="E368" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F368" t="n">

</xml_diff>

<commit_message>
Registro de pruebar diferentes funciones objetivos, falta encontrar la correcta
</commit_message>
<xml_diff>
--- a/src/PuLP/solucionOptima.xlsx
+++ b/src/PuLP/solucionOptima.xlsx
@@ -484,7 +484,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F2" t="n">
@@ -510,7 +510,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F3" t="n">
@@ -536,7 +536,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F4" t="n">
@@ -562,7 +562,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F5" t="n">
@@ -588,7 +588,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F6" t="n">
@@ -640,7 +640,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F8" t="n">
@@ -666,7 +666,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F9" t="n">
@@ -1316,7 +1316,7 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F34" t="n">
@@ -1342,7 +1342,7 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F35" t="n">
@@ -1446,7 +1446,7 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F39" t="n">
@@ -1472,7 +1472,7 @@
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F40" t="n">
@@ -1524,7 +1524,7 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F42" t="n">
@@ -1576,7 +1576,7 @@
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F44" t="n">
@@ -1602,7 +1602,7 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F45" t="n">
@@ -1628,7 +1628,7 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F46" t="n">
@@ -1654,7 +1654,7 @@
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F47" t="n">
@@ -1680,7 +1680,7 @@
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F48" t="n">
@@ -1706,7 +1706,7 @@
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F49" t="n">
@@ -1732,7 +1732,7 @@
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F50" t="n">
@@ -1758,7 +1758,7 @@
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F51" t="n">
@@ -1784,7 +1784,7 @@
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F52" t="n">
@@ -1810,7 +1810,7 @@
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F53" t="n">
@@ -1862,7 +1862,7 @@
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F55" t="n">
@@ -2382,7 +2382,7 @@
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F75" t="n">
@@ -2512,7 +2512,7 @@
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F80" t="n">
@@ -2564,7 +2564,7 @@
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F82" t="n">
@@ -2642,7 +2642,7 @@
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F85" t="n">
@@ -2668,7 +2668,7 @@
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F86" t="n">
@@ -2720,7 +2720,7 @@
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F88" t="n">
@@ -2772,7 +2772,7 @@
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F90" t="n">
@@ -2798,7 +2798,7 @@
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F91" t="n">
@@ -2824,7 +2824,7 @@
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F92" t="n">
@@ -2850,7 +2850,7 @@
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F93" t="n">
@@ -2876,7 +2876,7 @@
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F94" t="n">
@@ -2902,7 +2902,7 @@
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F95" t="n">
@@ -2928,7 +2928,7 @@
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F96" t="n">
@@ -2954,7 +2954,7 @@
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F97" t="n">
@@ -2980,7 +2980,7 @@
       </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F98" t="n">
@@ -3032,7 +3032,7 @@
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F100" t="n">
@@ -3058,7 +3058,7 @@
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F101" t="n">
@@ -3578,7 +3578,7 @@
       </c>
       <c r="E121" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F121" t="n">
@@ -3760,7 +3760,7 @@
       </c>
       <c r="E128" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F128" t="n">
@@ -3890,7 +3890,7 @@
       </c>
       <c r="E133" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F133" t="n">
@@ -3942,7 +3942,7 @@
       </c>
       <c r="E135" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F135" t="n">
@@ -3968,7 +3968,7 @@
       </c>
       <c r="E136" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F136" t="n">
@@ -3994,7 +3994,7 @@
       </c>
       <c r="E137" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F137" t="n">
@@ -4020,7 +4020,7 @@
       </c>
       <c r="E138" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F138" t="n">
@@ -4046,7 +4046,7 @@
       </c>
       <c r="E139" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F139" t="n">
@@ -4072,7 +4072,7 @@
       </c>
       <c r="E140" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F140" t="n">
@@ -4098,7 +4098,7 @@
       </c>
       <c r="E141" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F141" t="n">
@@ -4124,7 +4124,7 @@
       </c>
       <c r="E142" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F142" t="n">
@@ -4150,7 +4150,7 @@
       </c>
       <c r="E143" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F143" t="n">
@@ -4176,7 +4176,7 @@
       </c>
       <c r="E144" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F144" t="n">
@@ -4228,7 +4228,7 @@
       </c>
       <c r="E146" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F146" t="n">
@@ -4930,7 +4930,7 @@
       </c>
       <c r="E173" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F173" t="n">
@@ -4982,7 +4982,7 @@
       </c>
       <c r="E175" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F175" t="n">
@@ -5086,7 +5086,7 @@
       </c>
       <c r="E179" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F179" t="n">
@@ -5138,7 +5138,7 @@
       </c>
       <c r="E181" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F181" t="n">
@@ -5164,7 +5164,7 @@
       </c>
       <c r="E182" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F182" t="n">
@@ -5190,7 +5190,7 @@
       </c>
       <c r="E183" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F183" t="n">
@@ -5216,7 +5216,7 @@
       </c>
       <c r="E184" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F184" t="n">
@@ -5242,7 +5242,7 @@
       </c>
       <c r="E185" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F185" t="n">
@@ -5268,7 +5268,7 @@
       </c>
       <c r="E186" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F186" t="n">
@@ -5294,7 +5294,7 @@
       </c>
       <c r="E187" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F187" t="n">
@@ -5320,7 +5320,7 @@
       </c>
       <c r="E188" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F188" t="n">
@@ -5346,7 +5346,7 @@
       </c>
       <c r="E189" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F189" t="n">
@@ -5372,7 +5372,7 @@
       </c>
       <c r="E190" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F190" t="n">
@@ -5398,7 +5398,7 @@
       </c>
       <c r="E191" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F191" t="n">
@@ -5450,7 +5450,7 @@
       </c>
       <c r="E193" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F193" t="n">
@@ -5970,7 +5970,7 @@
       </c>
       <c r="E213" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F213" t="n">
@@ -6100,7 +6100,7 @@
       </c>
       <c r="E218" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F218" t="n">
@@ -6152,7 +6152,7 @@
       </c>
       <c r="E220" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F220" t="n">
@@ -6256,7 +6256,7 @@
       </c>
       <c r="E224" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F224" t="n">
@@ -6308,7 +6308,7 @@
       </c>
       <c r="E226" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F226" t="n">
@@ -6360,7 +6360,7 @@
       </c>
       <c r="E228" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F228" t="n">
@@ -6386,7 +6386,7 @@
       </c>
       <c r="E229" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F229" t="n">
@@ -6412,7 +6412,7 @@
       </c>
       <c r="E230" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F230" t="n">
@@ -6438,7 +6438,7 @@
       </c>
       <c r="E231" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F231" t="n">
@@ -6464,7 +6464,7 @@
       </c>
       <c r="E232" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F232" t="n">
@@ -6490,7 +6490,7 @@
       </c>
       <c r="E233" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F233" t="n">
@@ -6516,7 +6516,7 @@
       </c>
       <c r="E234" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F234" t="n">
@@ -6542,7 +6542,7 @@
       </c>
       <c r="E235" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F235" t="n">
@@ -6568,7 +6568,7 @@
       </c>
       <c r="E236" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F236" t="n">
@@ -6620,7 +6620,7 @@
       </c>
       <c r="E238" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F238" t="n">
@@ -6646,7 +6646,7 @@
       </c>
       <c r="E239" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F239" t="n">
@@ -7166,7 +7166,7 @@
       </c>
       <c r="E259" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F259" t="n">
@@ -7296,7 +7296,7 @@
       </c>
       <c r="E264" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F264" t="n">
@@ -7374,7 +7374,7 @@
       </c>
       <c r="E267" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F267" t="n">
@@ -7426,7 +7426,7 @@
       </c>
       <c r="E269" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F269" t="n">
@@ -7452,7 +7452,7 @@
       </c>
       <c r="E270" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F270" t="n">
@@ -7504,7 +7504,7 @@
       </c>
       <c r="E272" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F272" t="n">
@@ -7556,7 +7556,7 @@
       </c>
       <c r="E274" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F274" t="n">
@@ -7582,7 +7582,7 @@
       </c>
       <c r="E275" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F275" t="n">
@@ -7608,7 +7608,7 @@
       </c>
       <c r="E276" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F276" t="n">
@@ -7634,7 +7634,7 @@
       </c>
       <c r="E277" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F277" t="n">
@@ -7660,7 +7660,7 @@
       </c>
       <c r="E278" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F278" t="n">
@@ -7686,7 +7686,7 @@
       </c>
       <c r="E279" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F279" t="n">
@@ -7712,7 +7712,7 @@
       </c>
       <c r="E280" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F280" t="n">
@@ -7738,7 +7738,7 @@
       </c>
       <c r="E281" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F281" t="n">
@@ -7764,7 +7764,7 @@
       </c>
       <c r="E282" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F282" t="n">
@@ -7790,7 +7790,7 @@
       </c>
       <c r="E283" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F283" t="n">
@@ -7816,7 +7816,7 @@
       </c>
       <c r="E284" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F284" t="n">
@@ -8492,7 +8492,7 @@
       </c>
       <c r="E310" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F310" t="n">
@@ -8544,7 +8544,7 @@
       </c>
       <c r="E312" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F312" t="n">
@@ -8622,7 +8622,7 @@
       </c>
       <c r="E315" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F315" t="n">
@@ -8648,7 +8648,7 @@
       </c>
       <c r="E316" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F316" t="n">
@@ -8700,7 +8700,7 @@
       </c>
       <c r="E318" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F318" t="n">
@@ -8752,7 +8752,7 @@
       </c>
       <c r="E320" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F320" t="n">
@@ -8778,7 +8778,7 @@
       </c>
       <c r="E321" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F321" t="n">
@@ -8804,7 +8804,7 @@
       </c>
       <c r="E322" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F322" t="n">
@@ -8830,7 +8830,7 @@
       </c>
       <c r="E323" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F323" t="n">
@@ -8856,7 +8856,7 @@
       </c>
       <c r="E324" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F324" t="n">
@@ -8882,7 +8882,7 @@
       </c>
       <c r="E325" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F325" t="n">
@@ -8908,7 +8908,7 @@
       </c>
       <c r="E326" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F326" t="n">
@@ -8934,7 +8934,7 @@
       </c>
       <c r="E327" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F327" t="n">
@@ -8960,7 +8960,7 @@
       </c>
       <c r="E328" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F328" t="n">
@@ -8986,7 +8986,7 @@
       </c>
       <c r="E329" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F329" t="n">
@@ -9012,7 +9012,7 @@
       </c>
       <c r="E330" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F330" t="n">
@@ -9038,7 +9038,7 @@
       </c>
       <c r="E331" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F331" t="n">
@@ -9064,7 +9064,7 @@
       </c>
       <c r="E332" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F332" t="n">
@@ -9194,7 +9194,7 @@
       </c>
       <c r="E337" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F337" t="n">
@@ -9844,7 +9844,7 @@
       </c>
       <c r="E362" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F362" t="n">
@@ -9870,7 +9870,7 @@
       </c>
       <c r="E363" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F363" t="n">
@@ -9896,7 +9896,7 @@
       </c>
       <c r="E364" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F364" t="n">
@@ -9922,7 +9922,7 @@
       </c>
       <c r="E365" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F365" t="n">
@@ -9948,7 +9948,7 @@
       </c>
       <c r="E366" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F366" t="n">
@@ -9974,7 +9974,7 @@
       </c>
       <c r="E367" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F367" t="n">
@@ -10000,7 +10000,7 @@
       </c>
       <c r="E368" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F368" t="n">
@@ -10026,7 +10026,7 @@
       </c>
       <c r="E369" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F369" t="n">

</xml_diff>

<commit_message>
Posibles soluciones, están comentadas
</commit_message>
<xml_diff>
--- a/src/PuLP/solucionOptima.xlsx
+++ b/src/PuLP/solucionOptima.xlsx
@@ -614,7 +614,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F7" t="n">
@@ -744,7 +744,7 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F12" t="n">
@@ -1836,7 +1836,7 @@
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F54" t="n">
@@ -1862,7 +1862,7 @@
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F55" t="n">
@@ -2382,7 +2382,7 @@
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F75" t="n">
@@ -2512,7 +2512,7 @@
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F80" t="n">
@@ -3006,7 +3006,7 @@
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F99" t="n">
@@ -3110,7 +3110,7 @@
       </c>
       <c r="E103" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F103" t="n">
@@ -3578,7 +3578,7 @@
       </c>
       <c r="E121" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F121" t="n">
@@ -3708,7 +3708,7 @@
       </c>
       <c r="E126" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F126" t="n">
@@ -4202,7 +4202,7 @@
       </c>
       <c r="E145" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F145" t="n">
@@ -4904,7 +4904,7 @@
       </c>
       <c r="E172" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F172" t="n">
@@ -5424,7 +5424,7 @@
       </c>
       <c r="E192" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F192" t="n">
@@ -5528,7 +5528,7 @@
       </c>
       <c r="E196" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F196" t="n">
@@ -5970,7 +5970,7 @@
       </c>
       <c r="E213" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F213" t="n">
@@ -6100,7 +6100,7 @@
       </c>
       <c r="E218" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F218" t="n">
@@ -6594,7 +6594,7 @@
       </c>
       <c r="E237" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F237" t="n">
@@ -6698,7 +6698,7 @@
       </c>
       <c r="E241" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F241" t="n">
@@ -7166,7 +7166,7 @@
       </c>
       <c r="E259" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F259" t="n">
@@ -7296,7 +7296,7 @@
       </c>
       <c r="E264" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F264" t="n">
@@ -7842,7 +7842,7 @@
       </c>
       <c r="E285" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F285" t="n">
@@ -7920,7 +7920,7 @@
       </c>
       <c r="E288" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F288" t="n">
@@ -9194,7 +9194,7 @@
       </c>
       <c r="E337" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F337" t="n">
@@ -9220,7 +9220,7 @@
       </c>
       <c r="E338" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F338" t="n">
@@ -9714,7 +9714,7 @@
       </c>
       <c r="E357" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F357" t="n">
@@ -9818,7 +9818,7 @@
       </c>
       <c r="E361" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F361" t="n">

</xml_diff>

<commit_message>
Corregida funcion objetivo, lista las restricciones de las pausas activas, listo guardar el .csv
</commit_message>
<xml_diff>
--- a/src/PuLP/solucionOptima.xlsx
+++ b/src/PuLP/solucionOptima.xlsx
@@ -588,7 +588,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F6" t="n">
@@ -718,7 +718,7 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F11" t="n">
@@ -744,7 +744,7 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F12" t="n">
@@ -900,7 +900,7 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F18" t="n">
@@ -926,7 +926,7 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F19" t="n">
@@ -1056,7 +1056,7 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F24" t="n">
@@ -1082,7 +1082,7 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F25" t="n">
@@ -2018,7 +2018,7 @@
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F61" t="n">
@@ -2096,7 +2096,7 @@
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F64" t="n">
@@ -2122,7 +2122,7 @@
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F65" t="n">
@@ -2252,7 +2252,7 @@
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F70" t="n">
@@ -2278,7 +2278,7 @@
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F71" t="n">
@@ -2876,7 +2876,7 @@
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F94" t="n">
@@ -2902,7 +2902,7 @@
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F95" t="n">
@@ -3058,7 +3058,7 @@
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F101" t="n">
@@ -3110,7 +3110,7 @@
       </c>
       <c r="E103" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F103" t="n">
@@ -3578,7 +3578,7 @@
       </c>
       <c r="E121" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F121" t="n">
@@ -3864,7 +3864,7 @@
       </c>
       <c r="E132" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F132" t="n">
@@ -3890,7 +3890,7 @@
       </c>
       <c r="E133" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F133" t="n">
@@ -4072,7 +4072,7 @@
       </c>
       <c r="E140" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F140" t="n">
@@ -4098,7 +4098,7 @@
       </c>
       <c r="E141" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F141" t="n">
@@ -4800,7 +4800,7 @@
       </c>
       <c r="E168" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F168" t="n">
@@ -4904,7 +4904,7 @@
       </c>
       <c r="E172" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F172" t="n">
@@ -4930,7 +4930,7 @@
       </c>
       <c r="E173" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F173" t="n">
@@ -5060,7 +5060,7 @@
       </c>
       <c r="E178" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F178" t="n">
@@ -5086,7 +5086,7 @@
       </c>
       <c r="E179" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F179" t="n">
@@ -5268,7 +5268,7 @@
       </c>
       <c r="E186" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F186" t="n">
@@ -5294,7 +5294,7 @@
       </c>
       <c r="E187" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F187" t="n">
@@ -5450,7 +5450,7 @@
       </c>
       <c r="E193" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F193" t="n">
@@ -5528,7 +5528,7 @@
       </c>
       <c r="E196" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F196" t="n">
@@ -5970,7 +5970,7 @@
       </c>
       <c r="E213" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F213" t="n">
@@ -6256,7 +6256,7 @@
       </c>
       <c r="E224" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F224" t="n">
@@ -6282,7 +6282,7 @@
       </c>
       <c r="E225" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F225" t="n">
@@ -6464,7 +6464,7 @@
       </c>
       <c r="E232" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F232" t="n">
@@ -6490,7 +6490,7 @@
       </c>
       <c r="E233" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F233" t="n">
@@ -6646,7 +6646,7 @@
       </c>
       <c r="E239" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F239" t="n">
@@ -6698,7 +6698,7 @@
       </c>
       <c r="E241" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F241" t="n">
@@ -7244,7 +7244,7 @@
       </c>
       <c r="E262" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F262" t="n">
@@ -7296,7 +7296,7 @@
       </c>
       <c r="E264" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F264" t="n">
@@ -7374,7 +7374,7 @@
       </c>
       <c r="E267" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F267" t="n">
@@ -7452,7 +7452,7 @@
       </c>
       <c r="E270" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F270" t="n">
@@ -7478,7 +7478,7 @@
       </c>
       <c r="E271" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F271" t="n">
@@ -7660,7 +7660,7 @@
       </c>
       <c r="E278" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F278" t="n">
@@ -7686,7 +7686,7 @@
       </c>
       <c r="E279" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F279" t="n">
@@ -7842,7 +7842,7 @@
       </c>
       <c r="E285" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F285" t="n">
@@ -7920,7 +7920,7 @@
       </c>
       <c r="E288" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F288" t="n">
@@ -8336,7 +8336,7 @@
       </c>
       <c r="E304" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F304" t="n">
@@ -8466,7 +8466,7 @@
       </c>
       <c r="E309" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F309" t="n">
@@ -8492,7 +8492,7 @@
       </c>
       <c r="E310" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F310" t="n">
@@ -8648,7 +8648,7 @@
       </c>
       <c r="E316" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F316" t="n">
@@ -8674,7 +8674,7 @@
       </c>
       <c r="E317" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F317" t="n">
@@ -9220,7 +9220,7 @@
       </c>
       <c r="E338" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F338" t="n">
@@ -9272,7 +9272,7 @@
       </c>
       <c r="E340" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F340" t="n">
@@ -9792,7 +9792,7 @@
       </c>
       <c r="E360" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F360" t="n">
@@ -9818,7 +9818,7 @@
       </c>
       <c r="E361" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F361" t="n">

</xml_diff>

<commit_message>
Se arregló un error de código
</commit_message>
<xml_diff>
--- a/src/PuLP/solucionOptima.xlsx
+++ b/src/PuLP/solucionOptima.xlsx
@@ -588,7 +588,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F6" t="n">
@@ -666,7 +666,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F9" t="n">
@@ -718,7 +718,7 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F11" t="n">
@@ -900,7 +900,7 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F18" t="n">
@@ -926,7 +926,7 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F19" t="n">
@@ -1056,7 +1056,7 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F24" t="n">
@@ -1082,7 +1082,7 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F25" t="n">
@@ -1238,7 +1238,7 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F31" t="n">
@@ -1316,7 +1316,7 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F34" t="n">
@@ -2018,7 +2018,7 @@
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F61" t="n">
@@ -2096,7 +2096,7 @@
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F64" t="n">
@@ -2122,7 +2122,7 @@
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F65" t="n">
@@ -2252,7 +2252,7 @@
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F70" t="n">
@@ -2278,7 +2278,7 @@
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F71" t="n">
@@ -2434,7 +2434,7 @@
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F77" t="n">
@@ -2512,7 +2512,7 @@
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F80" t="n">
@@ -2876,7 +2876,7 @@
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F94" t="n">
@@ -2902,7 +2902,7 @@
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F95" t="n">
@@ -3578,7 +3578,7 @@
       </c>
       <c r="E121" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F121" t="n">
@@ -3630,7 +3630,7 @@
       </c>
       <c r="E123" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F123" t="n">
@@ -3708,7 +3708,7 @@
       </c>
       <c r="E126" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F126" t="n">
@@ -3864,7 +3864,7 @@
       </c>
       <c r="E132" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F132" t="n">
@@ -3890,7 +3890,7 @@
       </c>
       <c r="E133" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F133" t="n">
@@ -4072,7 +4072,7 @@
       </c>
       <c r="E140" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F140" t="n">
@@ -4098,7 +4098,7 @@
       </c>
       <c r="E141" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F141" t="n">
@@ -4800,7 +4800,7 @@
       </c>
       <c r="E168" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F168" t="n">
@@ -4852,7 +4852,7 @@
       </c>
       <c r="E170" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F170" t="n">
@@ -4930,7 +4930,7 @@
       </c>
       <c r="E173" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F173" t="n">
@@ -5060,7 +5060,7 @@
       </c>
       <c r="E178" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F178" t="n">
@@ -5086,7 +5086,7 @@
       </c>
       <c r="E179" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F179" t="n">
@@ -5268,7 +5268,7 @@
       </c>
       <c r="E186" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F186" t="n">
@@ -5294,7 +5294,7 @@
       </c>
       <c r="E187" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F187" t="n">
@@ -5450,7 +5450,7 @@
       </c>
       <c r="E193" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F193" t="n">
@@ -5476,7 +5476,7 @@
       </c>
       <c r="E194" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F194" t="n">
@@ -5684,7 +5684,7 @@
       </c>
       <c r="E202" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F202" t="n">
@@ -5840,7 +5840,7 @@
       </c>
       <c r="E208" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F208" t="n">
@@ -5970,7 +5970,7 @@
       </c>
       <c r="E213" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F213" t="n">
@@ -6074,7 +6074,7 @@
       </c>
       <c r="E217" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F217" t="n">
@@ -6100,7 +6100,7 @@
       </c>
       <c r="E218" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F218" t="n">
@@ -6256,7 +6256,7 @@
       </c>
       <c r="E224" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F224" t="n">
@@ -6282,7 +6282,7 @@
       </c>
       <c r="E225" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F225" t="n">
@@ -6490,7 +6490,7 @@
       </c>
       <c r="E233" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F233" t="n">
@@ -6646,7 +6646,7 @@
       </c>
       <c r="E239" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F239" t="n">
@@ -6698,7 +6698,7 @@
       </c>
       <c r="E241" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F241" t="n">
@@ -6880,7 +6880,7 @@
       </c>
       <c r="E248" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F248" t="n">
@@ -6906,7 +6906,7 @@
       </c>
       <c r="E249" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F249" t="n">
@@ -7036,7 +7036,7 @@
       </c>
       <c r="E254" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F254" t="n">
@@ -7062,7 +7062,7 @@
       </c>
       <c r="E255" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F255" t="n">
@@ -7244,7 +7244,7 @@
       </c>
       <c r="E262" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F262" t="n">
@@ -7296,7 +7296,7 @@
       </c>
       <c r="E264" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F264" t="n">
@@ -7374,7 +7374,7 @@
       </c>
       <c r="E267" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F267" t="n">
@@ -7478,7 +7478,7 @@
       </c>
       <c r="E271" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F271" t="n">
@@ -7842,7 +7842,7 @@
       </c>
       <c r="E285" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F285" t="n">
@@ -7920,7 +7920,7 @@
       </c>
       <c r="E288" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F288" t="n">
@@ -8076,7 +8076,7 @@
       </c>
       <c r="E294" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F294" t="n">
@@ -8102,7 +8102,7 @@
       </c>
       <c r="E295" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F295" t="n">
@@ -8128,7 +8128,7 @@
       </c>
       <c r="E296" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F296" t="n">
@@ -8232,7 +8232,7 @@
       </c>
       <c r="E300" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F300" t="n">
@@ -8258,7 +8258,7 @@
       </c>
       <c r="E301" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F301" t="n">
@@ -8284,7 +8284,7 @@
       </c>
       <c r="E302" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F302" t="n">
@@ -8336,7 +8336,7 @@
       </c>
       <c r="E304" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F304" t="n">
@@ -8466,7 +8466,7 @@
       </c>
       <c r="E309" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F309" t="n">
@@ -8492,7 +8492,7 @@
       </c>
       <c r="E310" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F310" t="n">

</xml_diff>

<commit_message>
Se bajó las iteraciones para mejoes resultados (Revisar por qué)
</commit_message>
<xml_diff>
--- a/src/PuLP/solucionOptima.xlsx
+++ b/src/PuLP/solucionOptima.xlsx
@@ -666,7 +666,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F9" t="n">
@@ -692,7 +692,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F10" t="n">
@@ -1862,7 +1862,7 @@
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F55" t="n">
@@ -1888,7 +1888,7 @@
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F56" t="n">
@@ -3058,7 +3058,7 @@
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F101" t="n">
@@ -3084,7 +3084,7 @@
       </c>
       <c r="E102" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F102" t="n">
@@ -3292,7 +3292,7 @@
       </c>
       <c r="E110" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F110" t="n">
@@ -3448,7 +3448,7 @@
       </c>
       <c r="E116" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F116" t="n">
@@ -4072,7 +4072,7 @@
       </c>
       <c r="E140" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F140" t="n">
@@ -4254,7 +4254,7 @@
       </c>
       <c r="E147" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F147" t="n">
@@ -4306,7 +4306,7 @@
       </c>
       <c r="E149" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F149" t="n">
@@ -4488,7 +4488,7 @@
       </c>
       <c r="E156" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F156" t="n">
@@ -4514,7 +4514,7 @@
       </c>
       <c r="E157" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F157" t="n">
@@ -4644,7 +4644,7 @@
       </c>
       <c r="E162" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F162" t="n">
@@ -4670,7 +4670,7 @@
       </c>
       <c r="E163" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F163" t="n">
@@ -4852,7 +4852,7 @@
       </c>
       <c r="E170" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F170" t="n">
@@ -4878,7 +4878,7 @@
       </c>
       <c r="E171" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F171" t="n">
@@ -5060,7 +5060,7 @@
       </c>
       <c r="E178" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F178" t="n">
@@ -5268,7 +5268,7 @@
       </c>
       <c r="E186" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F186" t="n">
@@ -5294,7 +5294,7 @@
       </c>
       <c r="E187" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F187" t="n">
@@ -5476,7 +5476,7 @@
       </c>
       <c r="E194" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F194" t="n">
@@ -5528,7 +5528,7 @@
       </c>
       <c r="E196" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F196" t="n">
@@ -5710,7 +5710,7 @@
       </c>
       <c r="E203" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F203" t="n">
@@ -5736,7 +5736,7 @@
       </c>
       <c r="E204" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F204" t="n">
@@ -5866,7 +5866,7 @@
       </c>
       <c r="E209" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F209" t="n">
@@ -5892,7 +5892,7 @@
       </c>
       <c r="E210" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F210" t="n">
@@ -6074,7 +6074,7 @@
       </c>
       <c r="E217" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F217" t="n">
@@ -6100,7 +6100,7 @@
       </c>
       <c r="E218" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F218" t="n">
@@ -6256,7 +6256,7 @@
       </c>
       <c r="E224" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F224" t="n">
@@ -6282,7 +6282,7 @@
       </c>
       <c r="E225" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F225" t="n">
@@ -6490,7 +6490,7 @@
       </c>
       <c r="E233" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F233" t="n">
@@ -6516,7 +6516,7 @@
       </c>
       <c r="E234" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F234" t="n">
@@ -6698,7 +6698,7 @@
       </c>
       <c r="E241" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F241" t="n">
@@ -6750,7 +6750,7 @@
       </c>
       <c r="E243" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F243" t="n">
@@ -6932,7 +6932,7 @@
       </c>
       <c r="E250" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F250" t="n">
@@ -6958,7 +6958,7 @@
       </c>
       <c r="E251" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F251" t="n">
@@ -7088,7 +7088,7 @@
       </c>
       <c r="E256" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F256" t="n">
@@ -7114,7 +7114,7 @@
       </c>
       <c r="E257" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F257" t="n">
@@ -7296,7 +7296,7 @@
       </c>
       <c r="E264" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F264" t="n">
@@ -7348,7 +7348,7 @@
       </c>
       <c r="E266" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F266" t="n">
@@ -7478,7 +7478,7 @@
       </c>
       <c r="E271" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F271" t="n">
@@ -7504,7 +7504,7 @@
       </c>
       <c r="E272" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F272" t="n">
@@ -7712,7 +7712,7 @@
       </c>
       <c r="E280" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F280" t="n">
@@ -7738,7 +7738,7 @@
       </c>
       <c r="E281" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F281" t="n">
@@ -7920,7 +7920,7 @@
       </c>
       <c r="E288" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F288" t="n">
@@ -7972,7 +7972,7 @@
       </c>
       <c r="E290" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F290" t="n">
@@ -8154,7 +8154,7 @@
       </c>
       <c r="E297" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F297" t="n">
@@ -8180,7 +8180,7 @@
       </c>
       <c r="E298" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F298" t="n">
@@ -8310,7 +8310,7 @@
       </c>
       <c r="E303" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F303" t="n">
@@ -8336,7 +8336,7 @@
       </c>
       <c r="E304" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F304" t="n">
@@ -8492,7 +8492,7 @@
       </c>
       <c r="E310" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F310" t="n">
@@ -8544,7 +8544,7 @@
       </c>
       <c r="E312" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F312" t="n">
@@ -8700,7 +8700,7 @@
       </c>
       <c r="E318" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F318" t="n">
@@ -8726,7 +8726,7 @@
       </c>
       <c r="E319" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F319" t="n">
@@ -9194,7 +9194,7 @@
       </c>
       <c r="E337" t="inlineStr">
         <is>
-          <t>Trabaja</t>
+          <t>Nada</t>
         </is>
       </c>
       <c r="F337" t="n">
@@ -9272,7 +9272,7 @@
       </c>
       <c r="E340" t="inlineStr">
         <is>
-          <t>Nada</t>
+          <t>Trabaja</t>
         </is>
       </c>
       <c r="F340" t="n">

</xml_diff>